<commit_message>
Theme 5 and Mooring import code
</commit_message>
<xml_diff>
--- a/data-lake/variable_key.xlsx
+++ b/data-lake/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\data-lake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29C4938-36D5-4A33-B51A-ECE7306D354B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668FDFC6-9708-42D6-BB99-2842996F4ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1040" windowWidth="14400" windowHeight="7590" activeTab="1" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
+    <workbookView xWindow="1380" yWindow="1380" windowWidth="14400" windowHeight="7590" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="DWER" sheetId="2" r:id="rId5"/>
     <sheet name="Information" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Key!$A$1:$H$181</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="848">
   <si>
     <t>Units</t>
   </si>
@@ -2571,6 +2574,18 @@
   </si>
   <si>
     <t>mmol /m^3</t>
+  </si>
+  <si>
+    <t>g kg-1</t>
+  </si>
+  <si>
+    <t>sea_water_salinity</t>
+  </si>
+  <si>
+    <t>sea_water_temperature</t>
+  </si>
+  <si>
+    <t>sea_water_turbidity</t>
   </si>
 </sst>
 </file>
@@ -3034,9 +3049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407D1833-63F5-4230-AD16-32E9E48F56BB}">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomLeft" activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3094,6 +3109,9 @@
       <c r="E2" s="1" t="s">
         <v>527</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -3111,6 +3129,9 @@
       <c r="E3" s="1" t="s">
         <v>528</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -3128,6 +3149,9 @@
       <c r="E4" s="1" t="s">
         <v>536</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -3145,6 +3169,9 @@
       <c r="E5" s="1" t="s">
         <v>537</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -3162,8 +3189,11 @@
       <c r="E6" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>211</v>
       </c>
@@ -3179,8 +3209,17 @@
       <c r="E7" s="1" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F7" s="17" t="s">
+        <v>845</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>212</v>
       </c>
@@ -3195,6 +3234,15 @@
       </c>
       <c r="E8" s="1" t="s">
         <v>530</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>846</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>702</v>
+      </c>
+      <c r="H8" s="1">
+        <v>-273.14999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -3213,6 +3261,9 @@
       <c r="E9" s="1" t="s">
         <v>531</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -3230,6 +3281,9 @@
       <c r="E10" s="1" t="s">
         <v>539</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -3247,6 +3301,9 @@
       <c r="E11" s="1" t="s">
         <v>540</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -3264,6 +3321,9 @@
       <c r="E12" s="1" t="s">
         <v>577</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -3281,8 +3341,11 @@
       <c r="E13" s="1" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>218</v>
       </c>
@@ -3297,6 +3360,15 @@
       </c>
       <c r="E14" s="1" t="s">
         <v>532</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>847</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -3315,6 +3387,9 @@
       <c r="E15" s="1" t="s">
         <v>694</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -3332,8 +3407,11 @@
       <c r="E16" s="1" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>221</v>
       </c>
@@ -3349,8 +3427,11 @@
       <c r="E17" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>222</v>
       </c>
@@ -3366,8 +3447,11 @@
       <c r="E18" s="1" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>223</v>
       </c>
@@ -3383,8 +3467,11 @@
       <c r="E19" s="1" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>224</v>
       </c>
@@ -3400,8 +3487,11 @@
       <c r="E20" s="1" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>225</v>
       </c>
@@ -3417,8 +3507,11 @@
       <c r="E21" s="1" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>226</v>
       </c>
@@ -3434,8 +3527,11 @@
       <c r="E22" s="1" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>227</v>
       </c>
@@ -3451,8 +3547,11 @@
       <c r="E23" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>228</v>
       </c>
@@ -3468,8 +3567,11 @@
       <c r="E24" s="1" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>229</v>
       </c>
@@ -3485,8 +3587,11 @@
       <c r="E25" s="1" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>230</v>
       </c>
@@ -3502,8 +3607,11 @@
       <c r="E26" s="1" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>231</v>
       </c>
@@ -3519,8 +3627,11 @@
       <c r="E27" s="1" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>232</v>
       </c>
@@ -3536,8 +3647,11 @@
       <c r="E28" s="1" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>233</v>
       </c>
@@ -3553,8 +3667,11 @@
       <c r="E29" s="1" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>234</v>
       </c>
@@ -3570,8 +3687,11 @@
       <c r="E30" s="1" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>235</v>
       </c>
@@ -3587,8 +3707,11 @@
       <c r="E31" s="1" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>236</v>
       </c>
@@ -3604,8 +3727,11 @@
       <c r="E32" s="1" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>237</v>
       </c>
@@ -3621,8 +3747,11 @@
       <c r="E33" s="1" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>238</v>
       </c>
@@ -3638,8 +3767,11 @@
       <c r="E34" s="1" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>239</v>
       </c>
@@ -3655,8 +3787,11 @@
       <c r="E35" s="1" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>240</v>
       </c>
@@ -3672,8 +3807,11 @@
       <c r="E36" s="1" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>241</v>
       </c>
@@ -3689,8 +3827,11 @@
       <c r="E37" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>242</v>
       </c>
@@ -3706,8 +3847,11 @@
       <c r="E38" s="1" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>243</v>
       </c>
@@ -3723,8 +3867,11 @@
       <c r="E39" s="1" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>244</v>
       </c>
@@ -3740,8 +3887,11 @@
       <c r="E40" s="1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>245</v>
       </c>
@@ -3757,8 +3907,11 @@
       <c r="E41" s="1" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>246</v>
       </c>
@@ -3774,8 +3927,11 @@
       <c r="E42" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>247</v>
       </c>
@@ -3791,8 +3947,11 @@
       <c r="E43" s="1" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>248</v>
       </c>
@@ -3808,8 +3967,11 @@
       <c r="E44" s="1" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>249</v>
       </c>
@@ -3825,8 +3987,11 @@
       <c r="E45" s="1" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>250</v>
       </c>
@@ -3842,8 +4007,11 @@
       <c r="E46" s="1" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>251</v>
       </c>
@@ -3859,8 +4027,11 @@
       <c r="E47" s="1" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>252</v>
       </c>
@@ -3876,8 +4047,11 @@
       <c r="E48" s="1" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>253</v>
       </c>
@@ -3893,8 +4067,11 @@
       <c r="E49" s="1" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>254</v>
       </c>
@@ -3907,8 +4084,11 @@
       <c r="E50" s="1" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>255</v>
       </c>
@@ -3921,8 +4101,11 @@
       <c r="E51" s="1" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>256</v>
       </c>
@@ -3935,8 +4118,11 @@
       <c r="E52" s="1" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>257</v>
       </c>
@@ -3949,8 +4135,11 @@
       <c r="E53" s="1" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>258</v>
       </c>
@@ -3963,8 +4152,11 @@
       <c r="E54" s="1" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>259</v>
       </c>
@@ -3980,8 +4172,11 @@
       <c r="E55" s="1" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>260</v>
       </c>
@@ -3994,8 +4189,11 @@
       <c r="E56" s="1" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>261</v>
       </c>
@@ -4008,8 +4206,11 @@
       <c r="E57" s="1" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>262</v>
       </c>
@@ -4022,8 +4223,11 @@
       <c r="E58" s="1" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>263</v>
       </c>
@@ -4036,8 +4240,11 @@
       <c r="E59" s="1" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>264</v>
       </c>
@@ -4050,8 +4257,11 @@
       <c r="E60" s="1" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>265</v>
       </c>
@@ -4064,8 +4274,11 @@
       <c r="E61" s="1" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>266</v>
       </c>
@@ -4078,8 +4291,11 @@
       <c r="E62" s="1" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>267</v>
       </c>
@@ -4092,8 +4308,11 @@
       <c r="E63" s="1" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>268</v>
       </c>
@@ -4106,8 +4325,11 @@
       <c r="E64" s="1" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>269</v>
       </c>
@@ -4120,8 +4342,11 @@
       <c r="E65" s="1" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>270</v>
       </c>
@@ -4134,8 +4359,11 @@
       <c r="E66" s="1" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>271</v>
       </c>
@@ -4148,8 +4376,11 @@
       <c r="E67" s="1" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>272</v>
       </c>
@@ -4162,8 +4393,11 @@
       <c r="E68" s="1" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>273</v>
       </c>
@@ -4176,8 +4410,11 @@
       <c r="E69" s="1" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>274</v>
       </c>
@@ -4190,8 +4427,11 @@
       <c r="E70" s="1" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>275</v>
       </c>
@@ -4204,8 +4444,11 @@
       <c r="E71" s="1" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>276</v>
       </c>
@@ -4218,8 +4461,11 @@
       <c r="E72" s="1" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>277</v>
       </c>
@@ -4232,8 +4478,11 @@
       <c r="E73" s="1" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>278</v>
       </c>
@@ -4246,8 +4495,11 @@
       <c r="E74" s="1" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>279</v>
       </c>
@@ -4260,8 +4512,11 @@
       <c r="E75" s="1" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>280</v>
       </c>
@@ -4274,8 +4529,11 @@
       <c r="E76" s="1" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>281</v>
       </c>
@@ -4288,8 +4546,11 @@
       <c r="E77" s="1" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>282</v>
       </c>
@@ -4302,8 +4563,11 @@
       <c r="E78" s="1" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>283</v>
       </c>
@@ -4316,8 +4580,11 @@
       <c r="E79" s="1" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>284</v>
       </c>
@@ -4330,8 +4597,11 @@
       <c r="E80" s="1" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>285</v>
       </c>
@@ -4344,8 +4614,11 @@
       <c r="E81" s="1" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>286</v>
       </c>
@@ -4358,8 +4631,11 @@
       <c r="E82" s="1" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>287</v>
       </c>
@@ -4372,8 +4648,11 @@
       <c r="E83" s="1" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>288</v>
       </c>
@@ -4386,8 +4665,11 @@
       <c r="E84" s="1" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>289</v>
       </c>
@@ -4400,8 +4682,11 @@
       <c r="E85" s="1" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>290</v>
       </c>
@@ -4414,8 +4699,11 @@
       <c r="E86" s="1" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>291</v>
       </c>
@@ -4428,8 +4716,11 @@
       <c r="E87" s="1" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>292</v>
       </c>
@@ -4442,8 +4733,11 @@
       <c r="E88" s="1" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>293</v>
       </c>
@@ -4456,8 +4750,11 @@
       <c r="E89" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>294</v>
       </c>
@@ -4470,8 +4767,11 @@
       <c r="E90" s="1" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>295</v>
       </c>
@@ -4484,8 +4784,11 @@
       <c r="E91" s="1" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>296</v>
       </c>
@@ -4498,8 +4801,11 @@
       <c r="E92" s="1" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>297</v>
       </c>
@@ -4512,8 +4818,11 @@
       <c r="E93" s="1" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>298</v>
       </c>
@@ -4526,8 +4835,11 @@
       <c r="E94" s="1" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>299</v>
       </c>
@@ -4540,8 +4852,11 @@
       <c r="E95" s="1" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>300</v>
       </c>
@@ -4554,8 +4869,11 @@
       <c r="E96" s="1" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>301</v>
       </c>
@@ -4568,8 +4886,11 @@
       <c r="E97" s="1" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>302</v>
       </c>
@@ -4582,8 +4903,11 @@
       <c r="E98" s="1" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>303</v>
       </c>
@@ -4596,8 +4920,11 @@
       <c r="E99" s="1" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>304</v>
       </c>
@@ -4610,8 +4937,11 @@
       <c r="E100" s="1" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>305</v>
       </c>
@@ -4624,8 +4954,11 @@
       <c r="E101" s="1" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>306</v>
       </c>
@@ -4638,8 +4971,11 @@
       <c r="E102" s="1" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>307</v>
       </c>
@@ -4652,8 +4988,11 @@
       <c r="E103" s="1" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>308</v>
       </c>
@@ -4666,8 +5005,11 @@
       <c r="E104" s="1" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>309</v>
       </c>
@@ -4680,8 +5022,11 @@
       <c r="E105" s="1" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>310</v>
       </c>
@@ -4694,8 +5039,11 @@
       <c r="E106" s="1" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>311</v>
       </c>
@@ -4708,8 +5056,11 @@
       <c r="E107" s="1" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>312</v>
       </c>
@@ -4722,8 +5073,11 @@
       <c r="E108" s="1" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>313</v>
       </c>
@@ -4736,8 +5090,11 @@
       <c r="E109" s="1" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F109" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>314</v>
       </c>
@@ -4750,8 +5107,11 @@
       <c r="E110" s="1" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>315</v>
       </c>
@@ -4764,8 +5124,11 @@
       <c r="E111" s="1" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F111" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>316</v>
       </c>
@@ -4778,8 +5141,11 @@
       <c r="E112" s="1" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F112" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -4792,8 +5158,11 @@
       <c r="E113" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F113" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>318</v>
       </c>
@@ -4806,8 +5175,11 @@
       <c r="E114" s="1" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F114" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>319</v>
       </c>
@@ -4820,8 +5192,11 @@
       <c r="E115" s="1" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>320</v>
       </c>
@@ -4834,8 +5209,11 @@
       <c r="E116" s="1" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F116" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>321</v>
       </c>
@@ -4848,8 +5226,11 @@
       <c r="E117" s="1" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F117" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>322</v>
       </c>
@@ -4862,8 +5243,11 @@
       <c r="E118" s="1" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>323</v>
       </c>
@@ -4876,8 +5260,11 @@
       <c r="E119" s="1" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>324</v>
       </c>
@@ -4890,8 +5277,11 @@
       <c r="E120" s="1" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>325</v>
       </c>
@@ -4904,8 +5294,11 @@
       <c r="E121" s="1" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F121" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>326</v>
       </c>
@@ -4918,8 +5311,11 @@
       <c r="E122" s="1" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F122" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>327</v>
       </c>
@@ -4932,8 +5328,11 @@
       <c r="E123" s="1" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F123" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>328</v>
       </c>
@@ -4946,8 +5345,11 @@
       <c r="E124" s="1" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F124" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>329</v>
       </c>
@@ -4960,8 +5362,11 @@
       <c r="E125" s="1" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F125" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>330</v>
       </c>
@@ -4974,8 +5379,11 @@
       <c r="E126" s="1" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F126" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>331</v>
       </c>
@@ -4988,8 +5396,11 @@
       <c r="E127" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F127" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>332</v>
       </c>
@@ -5001,6 +5412,9 @@
       </c>
       <c r="E128" s="1" t="s">
         <v>664</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -5016,6 +5430,9 @@
       <c r="E129" s="1" t="s">
         <v>665</v>
       </c>
+      <c r="F129" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="130" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
@@ -5073,6 +5490,9 @@
       <c r="E132" s="1" t="s">
         <v>695</v>
       </c>
+      <c r="F132" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
@@ -5090,6 +5510,9 @@
       <c r="E133" s="1" t="s">
         <v>696</v>
       </c>
+      <c r="F133" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
@@ -5104,6 +5527,9 @@
       <c r="E134" s="1" t="s">
         <v>550</v>
       </c>
+      <c r="F134" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
@@ -5118,6 +5544,9 @@
       <c r="E135" s="1" t="s">
         <v>566</v>
       </c>
+      <c r="F135" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
@@ -5132,6 +5561,9 @@
       <c r="E136" s="1" t="s">
         <v>551</v>
       </c>
+      <c r="F136" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
@@ -5149,6 +5581,9 @@
       <c r="E137" s="1" t="s">
         <v>574</v>
       </c>
+      <c r="F137" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
@@ -5163,6 +5598,9 @@
       <c r="E138" s="1" t="s">
         <v>567</v>
       </c>
+      <c r="F138" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
@@ -5177,6 +5615,9 @@
       <c r="E139" s="1" t="s">
         <v>552</v>
       </c>
+      <c r="F139" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
@@ -5194,6 +5635,9 @@
       <c r="E140" s="1" t="s">
         <v>553</v>
       </c>
+      <c r="F140" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="141" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
@@ -5225,6 +5669,9 @@
       <c r="E142" s="1" t="s">
         <v>555</v>
       </c>
+      <c r="F142" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
@@ -5239,6 +5686,9 @@
       <c r="E143" s="1" t="s">
         <v>556</v>
       </c>
+      <c r="F143" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
@@ -5253,6 +5703,9 @@
       <c r="E144" s="1" t="s">
         <v>557</v>
       </c>
+      <c r="F144" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
@@ -5267,6 +5720,9 @@
       <c r="E145" s="1" t="s">
         <v>558</v>
       </c>
+      <c r="F145" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
@@ -5281,6 +5737,9 @@
       <c r="E146" s="1" t="s">
         <v>568</v>
       </c>
+      <c r="F146" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
@@ -5295,6 +5754,9 @@
       <c r="E147" s="1" t="s">
         <v>666</v>
       </c>
+      <c r="F147" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
@@ -5309,6 +5771,9 @@
       <c r="E148" s="1" t="s">
         <v>667</v>
       </c>
+      <c r="F148" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
@@ -5323,6 +5788,9 @@
       <c r="E149" s="1" t="s">
         <v>668</v>
       </c>
+      <c r="F149" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
@@ -5337,6 +5805,9 @@
       <c r="E150" s="1" t="s">
         <v>625</v>
       </c>
+      <c r="F150" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
@@ -5351,6 +5822,9 @@
       <c r="E151" s="1" t="s">
         <v>626</v>
       </c>
+      <c r="F151" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
@@ -5365,6 +5839,9 @@
       <c r="E152" s="1" t="s">
         <v>627</v>
       </c>
+      <c r="F152" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
@@ -5379,6 +5856,9 @@
       <c r="E153" s="1" t="s">
         <v>569</v>
       </c>
+      <c r="F153" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="154" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
@@ -5493,6 +5973,9 @@
       <c r="E159" s="1" t="s">
         <v>670</v>
       </c>
+      <c r="F159" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
@@ -5507,8 +5990,11 @@
       <c r="E160" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F160" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>468</v>
       </c>
@@ -5521,8 +6007,11 @@
       <c r="E161" s="1" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F161" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>469</v>
       </c>
@@ -5535,8 +6024,11 @@
       <c r="E162" s="1" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F162" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>470</v>
       </c>
@@ -5549,8 +6041,11 @@
       <c r="E163" s="1" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F163" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>471</v>
       </c>
@@ -5563,8 +6058,11 @@
       <c r="E164" s="1" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F164" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>472</v>
       </c>
@@ -5577,8 +6075,11 @@
       <c r="E165" s="1" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F165" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>473</v>
       </c>
@@ -5591,8 +6092,11 @@
       <c r="E166" s="1" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F166" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>474</v>
       </c>
@@ -5605,8 +6109,11 @@
       <c r="E167" s="1" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F167" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>475</v>
       </c>
@@ -5619,8 +6126,11 @@
       <c r="E168" s="1" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F168" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>476</v>
       </c>
@@ -5633,8 +6143,11 @@
       <c r="E169" s="1" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F169" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>477</v>
       </c>
@@ -5647,8 +6160,11 @@
       <c r="E170" s="1" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F170" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>478</v>
       </c>
@@ -5661,8 +6177,11 @@
       <c r="E171" s="1" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F171" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>479</v>
       </c>
@@ -5675,8 +6194,11 @@
       <c r="E172" s="1" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F172" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>480</v>
       </c>
@@ -5686,8 +6208,11 @@
       <c r="E173" s="1" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F173" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>481</v>
       </c>
@@ -5700,8 +6225,11 @@
       <c r="E174" s="1" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F174" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>482</v>
       </c>
@@ -5714,8 +6242,11 @@
       <c r="E175" s="1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F175" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>483</v>
       </c>
@@ -5724,6 +6255,9 @@
       </c>
       <c r="E176" s="1" t="s">
         <v>685</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -5739,6 +6273,9 @@
       <c r="E177" s="1" t="s">
         <v>686</v>
       </c>
+      <c r="F177" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="178" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
@@ -5773,6 +6310,9 @@
       <c r="E179" s="1" t="s">
         <v>631</v>
       </c>
+      <c r="F179" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
@@ -5790,6 +6330,9 @@
       <c r="E180" s="1" t="s">
         <v>562</v>
       </c>
+      <c r="F180" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
@@ -5807,8 +6350,12 @@
       <c r="E181" s="1" t="s">
         <v>563</v>
       </c>
+      <c r="F181" s="1" t="s">
+        <v>841</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H181" xr:uid="{407D1833-63F5-4230-AD16-32E9E48F56BB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5819,7 +6366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3327CA4D-663D-443F-80DC-1A1E539BD38E}">
   <dimension ref="A1:F283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>

</xml_diff>